<commit_message>
Clean Up Excel Sheets
</commit_message>
<xml_diff>
--- a/Results Analysis/Results Analysis/Confusion Matrix Replication Results.xlsx
+++ b/Results Analysis/Results Analysis/Confusion Matrix Replication Results.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alerr\Documents\Masterarbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alerr\Documents\GitHub\replication-package\Results Analysis\Results Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8EF430-558E-4F29-95CB-D0ACA9FD41D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06E328B-0C5F-4F6C-8595-BA4897EA0292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C2440543-593E-4281-B627-232CF2608A65}"/>
   </bookViews>
   <sheets>
-    <sheet name="5-state confusion matrix (2)" sheetId="4" r:id="rId1"/>
-    <sheet name="2-state confusion matrix (2)" sheetId="3" r:id="rId2"/>
-    <sheet name="5-state confusion matrix" sheetId="2" r:id="rId3"/>
-    <sheet name="2-state confusion matrix" sheetId="1" r:id="rId4"/>
-    <sheet name="Tabelle1" sheetId="5" r:id="rId5"/>
+    <sheet name="5-state confusion matrix" sheetId="2" r:id="rId1"/>
+    <sheet name="2-state confusion matrix" sheetId="1" r:id="rId2"/>
+    <sheet name="Results Table" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Truth</t>
   </si>
@@ -288,23 +286,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -315,17 +304,17 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,18 +329,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -672,313 +649,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240A8EE1-905D-4A6E-A194-075705337A05}">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="12">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12">
-        <v>2</v>
-      </c>
-      <c r="D2" s="12">
-        <v>3</v>
-      </c>
-      <c r="E2" s="12">
-        <v>4</v>
-      </c>
-      <c r="F2" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>4.3</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>0.1</v>
-      </c>
-      <c r="E3">
-        <v>0.4</v>
-      </c>
-      <c r="F3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0.1</v>
-      </c>
-      <c r="C4">
-        <v>23.3</v>
-      </c>
-      <c r="D4">
-        <v>1.4</v>
-      </c>
-      <c r="E4">
-        <v>3.9</v>
-      </c>
-      <c r="F4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>5.8</v>
-      </c>
-      <c r="E5">
-        <v>1.2</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>12.1</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>5.4</v>
-      </c>
-      <c r="F6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6">
-        <v>2</v>
-      </c>
-      <c r="C7" s="6">
-        <v>4.8</v>
-      </c>
-      <c r="D7" s="6">
-        <v>2</v>
-      </c>
-      <c r="E7" s="6">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:F1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B3:F3">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:F4">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:F5">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6:F6">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:F7">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7735F305-46E4-46F4-906F-FB27F0C43324}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="28"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8">
-        <v>43.7</v>
-      </c>
-      <c r="C3" s="4">
-        <v>6.3</v>
-      </c>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9">
-        <v>12.9</v>
-      </c>
-      <c r="C4" s="6">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B3:C3">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:C4">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5561CD-16A8-4F2C-851D-9838F7CFD371}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -990,37 +664,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="21">
+      <c r="A2" s="22"/>
+      <c r="B2" s="12">
         <v>1</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="12">
         <v>2</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="12">
         <v>3</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="12">
         <v>4</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="12">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="13">
         <v>1</v>
       </c>
       <c r="B3">
@@ -1040,7 +714,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4">
@@ -1060,7 +734,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
       <c r="B5">
@@ -1080,7 +754,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
       <c r="B6">
@@ -1100,57 +774,57 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="A7" s="14">
         <v>5</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>2</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>4.8</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="11">
         <f>B12</f>
         <v>0.51497005988023958</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="11">
         <f t="shared" ref="C8:F8" si="0">C12</f>
         <v>0.9282868525896415</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="11">
         <f t="shared" si="0"/>
         <v>0.24999999999999992</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="11">
         <f t="shared" si="0"/>
         <v>0.44444444444444453</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1407,7 +1081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C15E83-BA78-4D6D-9AF4-F500FE85F30C}">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -1424,69 +1098,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="22"/>
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="4">
         <v>43.7</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>6.3</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="5">
         <v>12.9</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>19.100000000000001</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="7">
         <f>B10</f>
         <v>0.81988742964352723</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="11">
         <f>C10</f>
         <v>0.66550522648083632</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1615,105 +1289,105 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373F16F1-8549-4293-A88C-CC1901AA6AF7}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="34"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="18">
         <v>0.48</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="18">
         <v>13.1</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="19">
         <v>0.71</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="18">
         <v>0.11</v>
       </c>
-      <c r="G3" s="36">
+      <c r="G3" s="18">
         <v>16.399999999999999</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="20">
         <v>0.60980000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="18">
         <v>0.26</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="18">
         <v>14.8</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="19">
         <v>0.48</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="18">
         <v>0.22</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="18">
         <v>21.6</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="20">
         <v>0.35370000000000001</v>
       </c>
     </row>

</xml_diff>